<commit_message>
Manuscript first draft is finished, supplement still needs updates
</commit_message>
<xml_diff>
--- a/3_intermediate/OR_NS.xlsx
+++ b/3_intermediate/OR_NS.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="11505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="11505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="by_prov" sheetId="1" r:id="rId1"/>
+    <sheet name="all" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t>NFL &amp; NS</t>
   </si>
@@ -379,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,24 +582,68 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>3.33</v>
+      </c>
+      <c r="C2">
+        <v>2.78</v>
+      </c>
+      <c r="D2">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1.27</v>
+      </c>
+      <c r="C3">
+        <v>1.18</v>
+      </c>
+      <c r="D3">
+        <v>1.36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32c43fd1-a979-47d6-b9d5-576458252cc9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007B0FE2B274098644BBE49D8E4D13ECA6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="55403fdb8ec66b0f919cf9b41a22c461">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32c43fd1-a979-47d6-b9d5-576458252cc9" xmlns:ns4="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb94cb085d242424e051d5ac9bfaaae9" ns3:_="" ns4:_="">
     <xsd:import namespace="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
@@ -813,32 +858,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32c43fd1-a979-47d6-b9d5-576458252cc9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741AF563-0427-42FD-8047-356A09010DD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff"/>
-    <ds:schemaRef ds:uri="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01E67838-D539-4648-B05C-E09A4102F8B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ABB7319-D6BA-480A-8029-C6737FA64D3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -855,4 +892,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01E67838-D539-4648-B05C-E09A4102F8B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741AF563-0427-42FD-8047-356A09010DD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff"/>
+    <ds:schemaRef ds:uri="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated figures w new PSM model
</commit_message>
<xml_diff>
--- a/3_intermediate/OR_NS.xlsx
+++ b/3_intermediate/OR_NS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - McGill University\CLSA\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/jiacheng_chen_mcgill_ca/Documents/CLSA/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_9BC7E5E255895707AF537311436AD34F6CBBC73E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1FECD8F-A1A0-46FE-B923-BE592B820D62}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22905" windowHeight="11505" activeTab="1"/>
+    <workbookView xWindow="4590" yWindow="1215" windowWidth="21420" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="by_prov" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
   <si>
     <t>NFL &amp; NS</t>
   </si>
@@ -62,11 +63,14 @@
   <si>
     <t>BC</t>
   </si>
+  <si>
+    <t>Unweighted Analysis</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,11 +381,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,13 +416,13 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>3.75</v>
+        <v>3.04</v>
       </c>
       <c r="C2">
-        <v>2.31</v>
+        <v>1.84</v>
       </c>
       <c r="D2">
-        <v>6.35</v>
+        <v>5.25</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -429,13 +433,13 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1.38</v>
+        <v>1.34</v>
       </c>
       <c r="C3">
-        <v>1.18</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D3">
-        <v>1.61</v>
+        <v>1.59</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -446,13 +450,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>3.83</v>
+        <v>3.46</v>
       </c>
       <c r="C4">
-        <v>2.34</v>
+        <v>2.29</v>
       </c>
       <c r="D4">
-        <v>6.38</v>
+        <v>5.35</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -463,13 +467,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="C5">
-        <v>0.96</v>
+        <v>1.27</v>
       </c>
       <c r="D5">
-        <v>1.51</v>
+        <v>1.78</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -480,13 +484,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>3.4</v>
+        <v>4.03</v>
       </c>
       <c r="C6">
-        <v>2.4700000000000002</v>
+        <v>2.87</v>
       </c>
       <c r="D6">
-        <v>4.74</v>
+        <v>5.88</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -497,13 +501,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1.1200000000000001</v>
+        <v>1.42</v>
       </c>
       <c r="C7">
-        <v>0.98</v>
+        <v>1.23</v>
       </c>
       <c r="D7">
-        <v>1.29</v>
+        <v>1.65</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -514,13 +518,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2.0499999999999998</v>
+        <v>1.95</v>
       </c>
       <c r="C8">
-        <v>1.46</v>
+        <v>1.37</v>
       </c>
       <c r="D8">
-        <v>2.89</v>
+        <v>2.8</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -531,13 +535,13 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>1.48</v>
+        <v>1.49</v>
       </c>
       <c r="C9">
         <v>1.27</v>
       </c>
       <c r="D9">
-        <v>1.72</v>
+        <v>1.76</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -548,13 +552,13 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>4.9400000000000004</v>
+        <v>7.56</v>
       </c>
       <c r="C10">
-        <v>3.31</v>
+        <v>4.7300000000000004</v>
       </c>
       <c r="D10">
-        <v>7.64</v>
+        <v>12.8</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -565,13 +569,13 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>1.3</v>
+        <v>1.45</v>
       </c>
       <c r="C11">
-        <v>1.1200000000000001</v>
+        <v>1.24</v>
       </c>
       <c r="D11">
-        <v>1.51</v>
+        <v>1.7</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -583,11 +587,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,44 +602,73 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>3.33</v>
-      </c>
-      <c r="C2">
-        <v>2.78</v>
-      </c>
-      <c r="D2">
-        <v>4.01</v>
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>1.27</v>
-      </c>
-      <c r="C3">
-        <v>1.18</v>
-      </c>
-      <c r="D3">
-        <v>1.36</v>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>3.23</v>
+      </c>
+      <c r="C8">
+        <v>2.74</v>
+      </c>
+      <c r="D8">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1.37</v>
+      </c>
+      <c r="C9">
+        <v>1.28</v>
+      </c>
+      <c r="D9">
+        <v>1.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Codes cleaning - data cleaning & PSW
</commit_message>
<xml_diff>
--- a/3_intermediate/OR_NS.xlsx
+++ b/3_intermediate/OR_NS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/jiacheng_chen_mcgill_ca/Documents/CLSA/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_9BC7E5E255895707AF537311436AD34F6CBBC73E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1FECD8F-A1A0-46FE-B923-BE592B820D62}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_9BC7E5E255895707AF537311436AD34F6CBBC73E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E18466C2-4DFB-415D-BBB1-E25381BB15CF}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="1215" windowWidth="21420" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="435" windowWidth="21420" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="by_prov" sheetId="1" r:id="rId1"/>
@@ -416,13 +416,13 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>3.04</v>
+        <v>3.13</v>
       </c>
       <c r="C2">
-        <v>1.84</v>
+        <v>1.9</v>
       </c>
       <c r="D2">
-        <v>5.25</v>
+        <v>5.39</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -433,13 +433,13 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>1.34</v>
+        <v>1.4</v>
       </c>
       <c r="C3">
-        <v>1.1399999999999999</v>
+        <v>1.18</v>
       </c>
       <c r="D3">
-        <v>1.59</v>
+        <v>1.65</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
@@ -450,13 +450,13 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>3.46</v>
+        <v>3.26</v>
       </c>
       <c r="C4">
-        <v>2.29</v>
+        <v>2.16</v>
       </c>
       <c r="D4">
-        <v>5.35</v>
+        <v>5.01</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -467,13 +467,13 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>1.5</v>
+        <v>1.44</v>
       </c>
       <c r="C5">
-        <v>1.27</v>
+        <v>1.22</v>
       </c>
       <c r="D5">
-        <v>1.78</v>
+        <v>1.7</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -484,13 +484,13 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>4.03</v>
+        <v>4.1900000000000004</v>
       </c>
       <c r="C6">
-        <v>2.87</v>
+        <v>2.93</v>
       </c>
       <c r="D6">
-        <v>5.88</v>
+        <v>6.15</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -501,13 +501,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1.42</v>
+        <v>1.44</v>
       </c>
       <c r="C7">
-        <v>1.23</v>
+        <v>1.24</v>
       </c>
       <c r="D7">
-        <v>1.65</v>
+        <v>1.67</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -518,13 +518,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1.95</v>
+        <v>1.89</v>
       </c>
       <c r="C8">
-        <v>1.37</v>
+        <v>1.34</v>
       </c>
       <c r="D8">
-        <v>2.8</v>
+        <v>2.7</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -541,7 +541,7 @@
         <v>1.27</v>
       </c>
       <c r="D9">
-        <v>1.76</v>
+        <v>1.75</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -552,13 +552,13 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>7.56</v>
+        <v>7.26</v>
       </c>
       <c r="C10">
-        <v>4.7300000000000004</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="D10">
-        <v>12.8</v>
+        <v>12.4</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -569,13 +569,13 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>1.45</v>
+        <v>1.46</v>
       </c>
       <c r="C11">
-        <v>1.24</v>
+        <v>1.25</v>
       </c>
       <c r="D11">
-        <v>1.7</v>
+        <v>1.71</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -677,6 +677,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32c43fd1-a979-47d6-b9d5-576458252cc9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007B0FE2B274098644BBE49D8E4D13ECA6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="55403fdb8ec66b0f919cf9b41a22c461">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32c43fd1-a979-47d6-b9d5-576458252cc9" xmlns:ns4="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb94cb085d242424e051d5ac9bfaaae9" ns3:_="" ns4:_="">
     <xsd:import namespace="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
@@ -891,24 +908,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32c43fd1-a979-47d6-b9d5-576458252cc9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741AF563-0427-42FD-8047-356A09010DD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff"/>
+    <ds:schemaRef ds:uri="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01E67838-D539-4648-B05C-E09A4102F8B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ABB7319-D6BA-480A-8029-C6737FA64D3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -925,29 +950,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01E67838-D539-4648-B05C-E09A4102F8B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741AF563-0427-42FD-8047-356A09010DD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff"/>
-    <ds:schemaRef ds:uri="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated figs and tabs
</commit_message>
<xml_diff>
--- a/3_intermediate/OR_NS.xlsx
+++ b/3_intermediate/OR_NS.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/jiacheng_chen_mcgill_ca/Documents/CLSA/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udemontreal-my.sharepoint.com/personal/jiacheng_chen_1_umontreal_ca/Documents/Misc Proj/DBS vs Venous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_9BC7E5E255895707AF537311436AD34F6CBBC73E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E18466C2-4DFB-415D-BBB1-E25381BB15CF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA53F42C-18C2-46BA-94A6-161F11C693FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="435" windowWidth="21420" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3888" yWindow="1800" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="by_prov" sheetId="1" r:id="rId1"/>
-    <sheet name="all" sheetId="2" r:id="rId2"/>
+    <sheet name="by_prov" sheetId="3" r:id="rId1"/>
+    <sheet name="by_prov_old" sheetId="1" r:id="rId2"/>
+    <sheet name="all" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="15">
   <si>
     <t>NFL &amp; NS</t>
   </si>
@@ -65,18 +66,36 @@
   </si>
   <si>
     <t>Unweighted Analysis</t>
+  </si>
+  <si>
+    <t>MB &amp; AB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NL &amp; NS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -100,11 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -117,6 +137,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -381,16 +405,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE0E0283-A014-4C3B-9969-FF6DE9FE68A9}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -415,48 +439,48 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>3.13</v>
-      </c>
-      <c r="C2">
-        <v>1.9</v>
-      </c>
-      <c r="D2">
-        <v>5.39</v>
+      <c r="B2" s="1">
+        <v>0.31948881789137379</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.1855287569573284</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.52631578947368418</v>
       </c>
       <c r="E2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>1.4</v>
-      </c>
-      <c r="C3">
-        <v>1.18</v>
-      </c>
-      <c r="D3">
-        <v>1.65</v>
+      <c r="B3" s="1">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.60606060606060608</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.84745762711864414</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>3.26</v>
-      </c>
-      <c r="C4">
-        <v>2.16</v>
-      </c>
-      <c r="D4">
-        <v>5.01</v>
+      <c r="B4" s="1">
+        <v>0.30674846625766872</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.19960079840319361</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.46296296296296291</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -466,14 +490,14 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>1.44</v>
-      </c>
-      <c r="C5">
-        <v>1.22</v>
-      </c>
-      <c r="D5">
-        <v>1.7</v>
+      <c r="B5" s="1">
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.58823529411764708</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.81967213114754101</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -483,14 +507,14 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>4.1900000000000004</v>
-      </c>
-      <c r="C6">
-        <v>2.93</v>
-      </c>
-      <c r="D6">
-        <v>6.15</v>
+      <c r="B6" s="1">
+        <v>0.2386634844868735</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.16260162601626016</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.34129692832764502</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -500,14 +524,14 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>1.44</v>
-      </c>
-      <c r="C7">
-        <v>1.24</v>
-      </c>
-      <c r="D7">
-        <v>1.67</v>
+      <c r="B7" s="1">
+        <v>0.69444444444444442</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.5988023952095809</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.80645161290322587</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -517,48 +541,48 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>1.89</v>
-      </c>
-      <c r="C8">
-        <v>1.34</v>
-      </c>
-      <c r="D8">
-        <v>2.7</v>
+      <c r="B8" s="1">
+        <v>0.52910052910052918</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.37037037037037035</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.74626865671641784</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
-        <v>1.49</v>
-      </c>
-      <c r="C9">
-        <v>1.27</v>
-      </c>
-      <c r="D9">
-        <v>1.75</v>
+      <c r="B9" s="1">
+        <v>0.67114093959731547</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.78740157480314954</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
-        <v>7.26</v>
-      </c>
-      <c r="C10">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="D10">
-        <v>12.4</v>
+      <c r="B10" s="1">
+        <v>0.13774104683195593</v>
+      </c>
+      <c r="C10" s="1">
+        <v>8.0645161290322578E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.22123893805309736</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -568,6 +592,213 @@
       <c r="A11" t="s">
         <v>6</v>
       </c>
+      <c r="B11" s="1">
+        <v>0.68493150684931503</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.58479532163742687</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>3.13</v>
+      </c>
+      <c r="C2">
+        <v>1.9</v>
+      </c>
+      <c r="D2">
+        <v>5.39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>1.4</v>
+      </c>
+      <c r="C3">
+        <v>1.18</v>
+      </c>
+      <c r="D3">
+        <v>1.65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3.26</v>
+      </c>
+      <c r="C4">
+        <v>2.16</v>
+      </c>
+      <c r="D4">
+        <v>5.01</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>1.44</v>
+      </c>
+      <c r="C5">
+        <v>1.22</v>
+      </c>
+      <c r="D5">
+        <v>1.7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="C6">
+        <v>2.93</v>
+      </c>
+      <c r="D6">
+        <v>6.15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1.44</v>
+      </c>
+      <c r="C7">
+        <v>1.24</v>
+      </c>
+      <c r="D7">
+        <v>1.67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1.89</v>
+      </c>
+      <c r="C8">
+        <v>1.34</v>
+      </c>
+      <c r="D8">
+        <v>2.7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1.49</v>
+      </c>
+      <c r="C9">
+        <v>1.27</v>
+      </c>
+      <c r="D9">
+        <v>1.75</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>7.26</v>
+      </c>
+      <c r="C10">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D10">
+        <v>12.4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
       <c r="B11">
         <v>1.46</v>
       </c>
@@ -582,11 +813,12 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -594,10 +826,10 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,19 +904,12 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32c43fd1-a979-47d6-b9d5-576458252cc9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -693,7 +918,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007B0FE2B274098644BBE49D8E4D13ECA6" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="55403fdb8ec66b0f919cf9b41a22c461">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32c43fd1-a979-47d6-b9d5-576458252cc9" xmlns:ns4="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb94cb085d242424e051d5ac9bfaaae9" ns3:_="" ns4:_="">
     <xsd:import namespace="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
@@ -908,24 +1133,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32c43fd1-a979-47d6-b9d5-576458252cc9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741AF563-0427-42FD-8047-356A09010DD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff"/>
-    <ds:schemaRef ds:uri="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01E67838-D539-4648-B05C-E09A4102F8B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -933,7 +1149,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ABB7319-D6BA-480A-8029-C6737FA64D3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -950,4 +1166,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{741AF563-0427-42FD-8047-356A09010DD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ba23b94e-63d3-46d3-80f2-876b8fcbb7ff"/>
+    <ds:schemaRef ds:uri="32c43fd1-a979-47d6-b9d5-576458252cc9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>